<commit_message>
Trips/Travel index navigation sidebar ok & responsive
</commit_message>
<xml_diff>
--- a/app/assets/excel/MagicPeople.xlsx
+++ b/app/assets/excel/MagicPeople.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="253">
   <si>
     <t>Prénom</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>Benali</t>
+  </si>
+  <si>
+    <t>Nathalie</t>
+  </si>
+  <si>
+    <t>Benazet</t>
   </si>
   <si>
     <t>Siloé</t>
@@ -178,7 +184,7 @@
     <t>Caron</t>
   </si>
   <si>
-    <t>CHerbonnier</t>
+    <t>Cherbonnier</t>
   </si>
   <si>
     <t xml:space="preserve">Christian </t>
@@ -224,6 +230,12 @@
   </si>
   <si>
     <t>Demi</t>
+  </si>
+  <si>
+    <t>Johnny</t>
+  </si>
+  <si>
+    <t>Depp</t>
   </si>
   <si>
     <t xml:space="preserve">Antoine </t>
@@ -424,6 +436,18 @@
     <t>Hettich</t>
   </si>
   <si>
+    <t>Michel</t>
+  </si>
+  <si>
+    <t>Jobelot</t>
+  </si>
+  <si>
+    <t>Sébastien</t>
+  </si>
+  <si>
+    <t>Juste</t>
+  </si>
+  <si>
     <t>Benoit</t>
   </si>
   <si>
@@ -454,7 +478,7 @@
     <t>Lauvergeon</t>
   </si>
   <si>
-    <t>Marie et Ronan</t>
+    <t>Marie &amp; Ronan</t>
   </si>
   <si>
     <t>Le Fur</t>
@@ -481,7 +505,7 @@
     <t>Maxime</t>
   </si>
   <si>
-    <t xml:space="preserve">Louis seize </t>
+    <t xml:space="preserve">Louis-Seize </t>
   </si>
   <si>
     <t>Anne-Laure</t>
@@ -607,16 +631,13 @@
     <t>Pequin</t>
   </si>
   <si>
-    <t xml:space="preserve">Line </t>
-  </si>
-  <si>
     <t>Line</t>
   </si>
   <si>
     <t>Marion</t>
   </si>
   <si>
-    <t>Petit de mange</t>
+    <t>Petitdemange</t>
   </si>
   <si>
     <t xml:space="preserve">Thomas </t>
@@ -739,7 +760,7 @@
     <t>Velautham</t>
   </si>
   <si>
-    <t>Florence et Bruno</t>
+    <t>Florence &amp; Bruno</t>
   </si>
   <si>
     <t>Vuillemin</t>
@@ -835,7 +856,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -856,6 +877,12 @@
     </xf>
     <xf borderId="3" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -1563,10 +1590,10 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="2"/>
@@ -1850,11 +1877,11 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25" ht="20.25" customHeight="1">
-      <c r="A25" s="5" t="s">
+    <row r="25" ht="12.75" customHeight="1">
+      <c r="A25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="2"/>
@@ -1882,11 +1909,11 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="4" t="s">
+    <row r="26" ht="20.25" customHeight="1">
+      <c r="A26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C26" s="2"/>
@@ -2012,10 +2039,10 @@
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -2044,9 +2071,9 @@
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="2"/>
@@ -2175,7 +2202,7 @@
         <v>64</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2204,10 +2231,10 @@
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2331,10 +2358,10 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="7" t="s">
         <v>74</v>
       </c>
       <c r="C40" s="2"/>
@@ -2399,7 +2426,7 @@
         <v>77</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2428,10 +2455,10 @@
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2458,12 +2485,12 @@
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
     </row>
-    <row r="44" ht="20.25" customHeight="1">
-      <c r="A44" s="5" t="s">
+    <row r="44" ht="12.75" customHeight="1">
+      <c r="A44" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2522,11 +2549,11 @@
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
     </row>
-    <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="4" t="s">
+    <row r="46" ht="20.25" customHeight="1">
+      <c r="A46" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="6" t="s">
         <v>85</v>
       </c>
       <c r="C46" s="2"/>
@@ -2586,11 +2613,11 @@
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
     </row>
-    <row r="48" ht="20.25" customHeight="1">
-      <c r="A48" s="5" t="s">
+    <row r="48" ht="12.75" customHeight="1">
+      <c r="A48" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="4" t="s">
         <v>89</v>
       </c>
       <c r="C48" s="2"/>
@@ -2651,11 +2678,11 @@
       <c r="Z49" s="2"/>
     </row>
     <row r="50" ht="20.25" customHeight="1">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -2684,10 +2711,10 @@
     </row>
     <row r="51" ht="12.75" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -2714,12 +2741,12 @@
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
     </row>
-    <row r="52" ht="12.75" customHeight="1">
+    <row r="52" ht="20.25" customHeight="1">
       <c r="A52" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2748,10 +2775,10 @@
     </row>
     <row r="53" ht="12.75" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2780,10 +2807,10 @@
     </row>
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2812,7 +2839,7 @@
     </row>
     <row r="55" ht="12.75" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>101</v>
@@ -2906,11 +2933,11 @@
       <c r="Y57" s="2"/>
       <c r="Z57" s="2"/>
     </row>
-    <row r="58" ht="20.25" customHeight="1">
-      <c r="A58" s="5" t="s">
+    <row r="58" ht="12.75" customHeight="1">
+      <c r="A58" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="4" t="s">
         <v>107</v>
       </c>
       <c r="C58" s="2"/>
@@ -3034,11 +3061,11 @@
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
     </row>
-    <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="4" t="s">
+    <row r="62" ht="20.25" customHeight="1">
+      <c r="A62" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C62" s="2"/>
@@ -3100,10 +3127,10 @@
     </row>
     <row r="64" ht="12.75" customHeight="1">
       <c r="A64" s="4" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -3132,10 +3159,10 @@
     </row>
     <row r="65" ht="12.75" customHeight="1">
       <c r="A65" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -3164,7 +3191,7 @@
     </row>
     <row r="66" ht="12.75" customHeight="1">
       <c r="A66" s="4" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>122</v>
@@ -3226,11 +3253,11 @@
       <c r="Y67" s="2"/>
       <c r="Z67" s="2"/>
     </row>
-    <row r="68" ht="20.25" customHeight="1">
-      <c r="A68" s="5" t="s">
+    <row r="68" ht="12.75" customHeight="1">
+      <c r="A68" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="4" t="s">
         <v>126</v>
       </c>
       <c r="C68" s="2"/>
@@ -3324,10 +3351,10 @@
     </row>
     <row r="71" ht="12.75" customHeight="1">
       <c r="A71" s="4" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -3354,12 +3381,12 @@
       <c r="Y71" s="2"/>
       <c r="Z71" s="2"/>
     </row>
-    <row r="72" ht="12.75" customHeight="1">
-      <c r="A72" s="4" t="s">
-        <v>131</v>
+    <row r="72" ht="20.25" customHeight="1">
+      <c r="A72" s="5" t="s">
+        <v>133</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>132</v>
+      <c r="B72" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -3388,7 +3415,7 @@
     </row>
     <row r="73" ht="12.75" customHeight="1">
       <c r="A73" s="4" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>134</v>
@@ -3515,10 +3542,10 @@
       <c r="Z76" s="2"/>
     </row>
     <row r="77" ht="12.75" customHeight="1">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="7" t="s">
         <v>142</v>
       </c>
       <c r="C77" s="2"/>
@@ -3547,10 +3574,10 @@
       <c r="Z77" s="2"/>
     </row>
     <row r="78" ht="12.75" customHeight="1">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="7" t="s">
         <v>144</v>
       </c>
       <c r="C78" s="2"/>
@@ -3578,11 +3605,11 @@
       <c r="Y78" s="2"/>
       <c r="Z78" s="2"/>
     </row>
-    <row r="79" ht="20.25" customHeight="1">
-      <c r="A79" s="5" t="s">
+    <row r="79" ht="12.75" customHeight="1">
+      <c r="A79" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="4" t="s">
         <v>146</v>
       </c>
       <c r="C79" s="2"/>
@@ -3610,11 +3637,11 @@
       <c r="Y79" s="2"/>
       <c r="Z79" s="2"/>
     </row>
-    <row r="80" ht="20.25" customHeight="1">
-      <c r="A80" s="5" t="s">
+    <row r="80" ht="12.75" customHeight="1">
+      <c r="A80" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="4" t="s">
         <v>148</v>
       </c>
       <c r="C80" s="2"/>
@@ -3676,10 +3703,10 @@
     </row>
     <row r="82" ht="12.75" customHeight="1">
       <c r="A82" s="4" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
@@ -3706,12 +3733,12 @@
       <c r="Y82" s="2"/>
       <c r="Z82" s="2"/>
     </row>
-    <row r="83" ht="12.75" customHeight="1">
-      <c r="A83" s="4" t="s">
-        <v>33</v>
+    <row r="83" ht="20.25" customHeight="1">
+      <c r="A83" s="5" t="s">
+        <v>153</v>
       </c>
-      <c r="B83" s="4" t="s">
-        <v>152</v>
+      <c r="B83" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
@@ -3738,12 +3765,12 @@
       <c r="Y83" s="2"/>
       <c r="Z83" s="2"/>
     </row>
-    <row r="84" ht="12.75" customHeight="1">
-      <c r="A84" s="4" t="s">
-        <v>153</v>
+    <row r="84" ht="20.25" customHeight="1">
+      <c r="A84" s="8" t="s">
+        <v>155</v>
       </c>
-      <c r="B84" s="4" t="s">
-        <v>154</v>
+      <c r="B84" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -3772,10 +3799,10 @@
     </row>
     <row r="85" ht="12.75" customHeight="1">
       <c r="A85" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>156</v>
+      <c r="B85" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
@@ -3804,10 +3831,10 @@
     </row>
     <row r="86" ht="12.75" customHeight="1">
       <c r="A86" s="4" t="s">
-        <v>157</v>
+        <v>112</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
@@ -3836,10 +3863,10 @@
     </row>
     <row r="87" ht="12.75" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
@@ -3868,10 +3895,10 @@
     </row>
     <row r="88" ht="12.75" customHeight="1">
       <c r="A88" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
@@ -3900,10 +3927,10 @@
     </row>
     <row r="89" ht="12.75" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
-      <c r="B89" s="4" t="s">
-        <v>162</v>
+      <c r="B89" s="7" t="s">
+        <v>164</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -3932,10 +3959,10 @@
     </row>
     <row r="90" ht="12.75" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
@@ -3964,10 +3991,10 @@
     </row>
     <row r="91" ht="12.75" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>165</v>
+        <v>62</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
@@ -3996,10 +4023,10 @@
     </row>
     <row r="92" ht="12.75" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -4028,10 +4055,10 @@
     </row>
     <row r="93" ht="12.75" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>31</v>
+        <v>169</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
@@ -4060,10 +4087,10 @@
     </row>
     <row r="94" ht="12.75" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
@@ -4092,10 +4119,10 @@
     </row>
     <row r="95" ht="12.75" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -4124,10 +4151,10 @@
     </row>
     <row r="96" ht="12.75" customHeight="1">
       <c r="A96" s="4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -4156,10 +4183,10 @@
     </row>
     <row r="97" ht="12.75" customHeight="1">
       <c r="A97" s="4" t="s">
-        <v>174</v>
+        <v>33</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
@@ -4188,10 +4215,10 @@
     </row>
     <row r="98" ht="12.75" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
@@ -4250,11 +4277,11 @@
       <c r="Y99" s="2"/>
       <c r="Z99" s="2"/>
     </row>
-    <row r="100" ht="20.25" customHeight="1">
-      <c r="A100" s="5" t="s">
+    <row r="100" ht="12.75" customHeight="1">
+      <c r="A100" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B100" s="6" t="s">
+      <c r="B100" s="4" t="s">
         <v>181</v>
       </c>
       <c r="C100" s="2"/>
@@ -4316,10 +4343,10 @@
     </row>
     <row r="102" ht="12.75" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>35</v>
+        <v>184</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
@@ -4348,10 +4375,10 @@
     </row>
     <row r="103" ht="12.75" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
@@ -4378,12 +4405,12 @@
       <c r="Y103" s="2"/>
       <c r="Z103" s="2"/>
     </row>
-    <row r="104" ht="12.75" customHeight="1">
-      <c r="A104" s="4" t="s">
-        <v>187</v>
+    <row r="104" ht="20.25" customHeight="1">
+      <c r="A104" s="5" t="s">
+        <v>188</v>
       </c>
-      <c r="B104" s="4" t="s">
-        <v>188</v>
+      <c r="B104" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
@@ -4412,10 +4439,10 @@
     </row>
     <row r="105" ht="12.75" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
@@ -4444,7 +4471,7 @@
     </row>
     <row r="106" ht="12.75" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>191</v>
+        <v>37</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>192</v>
@@ -4540,10 +4567,10 @@
     </row>
     <row r="109" ht="12.75" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -4572,10 +4599,10 @@
     </row>
     <row r="110" ht="12.75" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
@@ -4604,10 +4631,10 @@
     </row>
     <row r="111" ht="12.75" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
@@ -4636,10 +4663,10 @@
     </row>
     <row r="112" ht="12.75" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
@@ -4668,10 +4695,10 @@
     </row>
     <row r="113" ht="12.75" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>77</v>
+        <v>177</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -4700,10 +4727,10 @@
     </row>
     <row r="114" ht="12.75" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -4732,7 +4759,7 @@
     </row>
     <row r="115" ht="12.75" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>205</v>
@@ -4764,10 +4791,10 @@
     </row>
     <row r="116" ht="12.75" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
-      <c r="B116" s="4" t="s">
-        <v>206</v>
+      <c r="B116" s="7" t="s">
+        <v>208</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
@@ -4796,10 +4823,10 @@
     </row>
     <row r="117" ht="12.75" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
@@ -4828,10 +4855,10 @@
     </row>
     <row r="118" ht="12.75" customHeight="1">
       <c r="A118" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
@@ -4860,10 +4887,10 @@
     </row>
     <row r="119" ht="12.75" customHeight="1">
       <c r="A119" s="4" t="s">
-        <v>211</v>
+        <v>75</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
@@ -4890,12 +4917,12 @@
       <c r="Y119" s="2"/>
       <c r="Z119" s="2"/>
     </row>
-    <row r="120" ht="20.25" customHeight="1">
-      <c r="A120" s="5" t="s">
-        <v>213</v>
+    <row r="120" ht="12.75" customHeight="1">
+      <c r="A120" s="4" t="s">
+        <v>214</v>
       </c>
-      <c r="B120" s="6" t="s">
-        <v>214</v>
+      <c r="B120" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
@@ -4924,10 +4951,10 @@
     </row>
     <row r="121" ht="12.75" customHeight="1">
       <c r="A121" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -4956,10 +4983,10 @@
     </row>
     <row r="122" ht="12.75" customHeight="1">
       <c r="A122" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
@@ -4988,10 +5015,10 @@
     </row>
     <row r="123" ht="20.25" customHeight="1">
       <c r="A123" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
@@ -5020,10 +5047,10 @@
     </row>
     <row r="124" ht="12.75" customHeight="1">
       <c r="A124" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
@@ -5052,10 +5079,10 @@
     </row>
     <row r="125" ht="12.75" customHeight="1">
       <c r="A125" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
@@ -5082,12 +5109,12 @@
       <c r="Y125" s="2"/>
       <c r="Z125" s="2"/>
     </row>
-    <row r="126" ht="12.75" customHeight="1">
-      <c r="A126" s="4" t="s">
-        <v>225</v>
+    <row r="126" ht="20.25" customHeight="1">
+      <c r="A126" s="5" t="s">
+        <v>226</v>
       </c>
-      <c r="B126" s="4" t="s">
-        <v>226</v>
+      <c r="B126" s="6" t="s">
+        <v>227</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
@@ -5116,10 +5143,10 @@
     </row>
     <row r="127" ht="12.75" customHeight="1">
       <c r="A127" s="4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
@@ -5148,10 +5175,10 @@
     </row>
     <row r="128" ht="12.75" customHeight="1">
       <c r="A128" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
@@ -5180,10 +5207,10 @@
     </row>
     <row r="129" ht="12.75" customHeight="1">
       <c r="A129" s="4" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
@@ -5212,10 +5239,10 @@
     </row>
     <row r="130" ht="12.75" customHeight="1">
       <c r="A130" s="4" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
@@ -5244,10 +5271,10 @@
     </row>
     <row r="131" ht="12.75" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>77</v>
+        <v>236</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
@@ -5276,10 +5303,10 @@
     </row>
     <row r="132" ht="12.75" customHeight="1">
       <c r="A132" s="4" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
@@ -5308,10 +5335,10 @@
     </row>
     <row r="133" ht="12.75" customHeight="1">
       <c r="A133" s="4" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
@@ -5340,10 +5367,10 @@
     </row>
     <row r="134" ht="12.75" customHeight="1">
       <c r="A134" s="4" t="s">
-        <v>238</v>
+        <v>81</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
@@ -5372,7 +5399,7 @@
     </row>
     <row r="135" ht="12.75" customHeight="1">
       <c r="A135" s="4" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>241</v>
@@ -5402,12 +5429,12 @@
       <c r="Y135" s="2"/>
       <c r="Z135" s="2"/>
     </row>
-    <row r="136" ht="20.25" customHeight="1">
-      <c r="A136" s="5" t="s">
-        <v>242</v>
+    <row r="136" ht="12.75" customHeight="1">
+      <c r="A136" s="4" t="s">
+        <v>243</v>
       </c>
-      <c r="B136" s="6" t="s">
-        <v>243</v>
+      <c r="B136" s="4" t="s">
+        <v>244</v>
       </c>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
@@ -5436,10 +5463,10 @@
     </row>
     <row r="137" ht="12.75" customHeight="1">
       <c r="A137" s="4" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
@@ -5468,9 +5495,11 @@
     </row>
     <row r="138" ht="12.75" customHeight="1">
       <c r="A138" s="4" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
-      <c r="B138" s="7"/>
+      <c r="B138" s="4" t="s">
+        <v>248</v>
+      </c>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
@@ -5496,9 +5525,13 @@
       <c r="Y138" s="2"/>
       <c r="Z138" s="2"/>
     </row>
-    <row r="139" ht="18.0" customHeight="1">
-      <c r="A139" s="2"/>
-      <c r="B139" s="2"/>
+    <row r="139" ht="20.25" customHeight="1">
+      <c r="A139" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>250</v>
+      </c>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
@@ -5524,9 +5557,13 @@
       <c r="Y139" s="2"/>
       <c r="Z139" s="2"/>
     </row>
-    <row r="140" ht="18.0" customHeight="1">
-      <c r="A140" s="2"/>
-      <c r="B140" s="2"/>
+    <row r="140" ht="12.75" customHeight="1">
+      <c r="A140" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>250</v>
+      </c>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
@@ -5552,9 +5589,11 @@
       <c r="Y140" s="2"/>
       <c r="Z140" s="2"/>
     </row>
-    <row r="141" ht="18.0" customHeight="1">
-      <c r="A141" s="2"/>
-      <c r="B141" s="2"/>
+    <row r="141" ht="12.75" customHeight="1">
+      <c r="A141" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B141" s="9"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
@@ -29632,6 +29671,90 @@
       <c r="Y1000" s="2"/>
       <c r="Z1000" s="2"/>
     </row>
+    <row r="1001" ht="18.0" customHeight="1">
+      <c r="A1001" s="2"/>
+      <c r="B1001" s="2"/>
+      <c r="C1001" s="2"/>
+      <c r="D1001" s="2"/>
+      <c r="E1001" s="2"/>
+      <c r="F1001" s="2"/>
+      <c r="G1001" s="2"/>
+      <c r="H1001" s="2"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="2"/>
+      <c r="K1001" s="2"/>
+      <c r="L1001" s="2"/>
+      <c r="M1001" s="2"/>
+      <c r="N1001" s="2"/>
+      <c r="O1001" s="2"/>
+      <c r="P1001" s="2"/>
+      <c r="Q1001" s="2"/>
+      <c r="R1001" s="2"/>
+      <c r="S1001" s="2"/>
+      <c r="T1001" s="2"/>
+      <c r="U1001" s="2"/>
+      <c r="V1001" s="2"/>
+      <c r="W1001" s="2"/>
+      <c r="X1001" s="2"/>
+      <c r="Y1001" s="2"/>
+      <c r="Z1001" s="2"/>
+    </row>
+    <row r="1002" ht="18.0" customHeight="1">
+      <c r="A1002" s="2"/>
+      <c r="B1002" s="2"/>
+      <c r="C1002" s="2"/>
+      <c r="D1002" s="2"/>
+      <c r="E1002" s="2"/>
+      <c r="F1002" s="2"/>
+      <c r="G1002" s="2"/>
+      <c r="H1002" s="2"/>
+      <c r="I1002" s="2"/>
+      <c r="J1002" s="2"/>
+      <c r="K1002" s="2"/>
+      <c r="L1002" s="2"/>
+      <c r="M1002" s="2"/>
+      <c r="N1002" s="2"/>
+      <c r="O1002" s="2"/>
+      <c r="P1002" s="2"/>
+      <c r="Q1002" s="2"/>
+      <c r="R1002" s="2"/>
+      <c r="S1002" s="2"/>
+      <c r="T1002" s="2"/>
+      <c r="U1002" s="2"/>
+      <c r="V1002" s="2"/>
+      <c r="W1002" s="2"/>
+      <c r="X1002" s="2"/>
+      <c r="Y1002" s="2"/>
+      <c r="Z1002" s="2"/>
+    </row>
+    <row r="1003" ht="18.0" customHeight="1">
+      <c r="A1003" s="2"/>
+      <c r="B1003" s="2"/>
+      <c r="C1003" s="2"/>
+      <c r="D1003" s="2"/>
+      <c r="E1003" s="2"/>
+      <c r="F1003" s="2"/>
+      <c r="G1003" s="2"/>
+      <c r="H1003" s="2"/>
+      <c r="I1003" s="2"/>
+      <c r="J1003" s="2"/>
+      <c r="K1003" s="2"/>
+      <c r="L1003" s="2"/>
+      <c r="M1003" s="2"/>
+      <c r="N1003" s="2"/>
+      <c r="O1003" s="2"/>
+      <c r="P1003" s="2"/>
+      <c r="Q1003" s="2"/>
+      <c r="R1003" s="2"/>
+      <c r="S1003" s="2"/>
+      <c r="T1003" s="2"/>
+      <c r="U1003" s="2"/>
+      <c r="V1003" s="2"/>
+      <c r="W1003" s="2"/>
+      <c r="X1003" s="2"/>
+      <c r="Y1003" s="2"/>
+      <c r="Z1003" s="2"/>
+    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="1.0" right="1.0" top="1.0"/>

</xml_diff>